<commit_message>
Ensure csv and xlsx FAIR data + corrections
</commit_message>
<xml_diff>
--- a/FAIR_output_data/Experiment 1/Experiment 1 - bird dispersal - perlin noise with 2 x 10^5 m^2 patches.xlsx
+++ b/FAIR_output_data/Experiment 1/Experiment 1 - bird dispersal - perlin noise with 2 x 10^5 m^2 patches.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Development\DBR-sim\FAIR_output_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Development\DBR-sim\FAIR_output_data\Experiment 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA4F76F-A97F-4321-88D6-3B9D0F1947EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C003C5D-13C3-47BF-B632-F08672A76125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{69E6BE2E-CE5A-4BD2-A80A-851DDA8B992B}"/>
+    <workbookView xWindow="28680" yWindow="1620" windowWidth="29040" windowHeight="15720" xr2:uid="{69E6BE2E-CE5A-4BD2-A80A-851DDA8B992B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67CF6B2D-695A-4B34-A670-7EB8E85D92B6}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,15 +479,16 @@
     <col min="2" max="2" width="42.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0.1</v>
       </c>
@@ -495,7 +496,7 @@
         <v>0.58550862784073998</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.21</v>
       </c>
@@ -503,7 +504,7 @@
         <v>0.77485818127544204</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.32</v>
       </c>
@@ -511,7 +512,7 @@
         <v>0.94380889169753102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.43</v>
       </c>
@@ -519,7 +520,7 @@
         <v>1.11457186700501</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0.54</v>
       </c>
@@ -527,7 +528,7 @@
         <v>1.45836614076715</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>0.65</v>
       </c>
@@ -535,7 +536,7 @@
         <v>2.0659104269577</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>0.76</v>
       </c>
@@ -543,7 +544,7 @@
         <v>2.6259890000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>0.87</v>
       </c>
@@ -551,7 +552,7 @@
         <v>3.9518</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>0.9</v>
       </c>

</xml_diff>